<commit_message>
hecking out some new data
</commit_message>
<xml_diff>
--- a/WeatherStationsforProj2.xlsx
+++ b/WeatherStationsforProj2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kahme\Desktop\Project-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NBLaptop/Documents/Proj2Stuff/Project-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1943D7EF-F283-4FD9-9215-4D422CE39C5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C175C9F-AC7A-D440-A743-1089BA28DA5A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B4A3FB93-17A3-E44A-9EF5-4D288C62B5D6}"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="26340" windowHeight="13340" xr2:uid="{B4A3FB93-17A3-E44A-9EF5-4D288C62B5D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Detroit:</t>
   </si>
@@ -95,6 +95,9 @@
     <t>Anchorage:</t>
   </si>
   <si>
+    <t>Honolulu:</t>
+  </si>
+  <si>
     <t>Corpus Christi:</t>
   </si>
   <si>
@@ -117,6 +120,9 @@
   </si>
   <si>
     <t>USW00012924</t>
+  </si>
+  <si>
+    <t>USW00022521</t>
   </si>
   <si>
     <t>USC00500275</t>
@@ -580,13 +586,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1181BEA-3CE5-9244-90DF-7BC99B3575F2}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:B18"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
@@ -594,7 +600,7 @@
     <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,18 +611,18 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -633,36 +639,36 @@
         <v>12</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -673,151 +679,162 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>28</v>
+      <c r="B18" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>